<commit_message>
data source blujay and forecast
</commit_message>
<xml_diff>
--- a/reference/sales_report/FORECAST_BULK_2022.xlsx
+++ b/reference/sales_report/FORECAST_BULK_2022.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="32">
   <si>
     <t>SALES_NAME</t>
   </si>
@@ -124,6 +124,9 @@
   </si>
   <si>
     <t>CLARIANT</t>
+  </si>
+  <si>
+    <t>SUMBER HASIL PRIMA</t>
   </si>
 </sst>
 </file>
@@ -493,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q88"/>
+  <dimension ref="A1:Q86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -581,41 +584,17 @@
       <c r="E2" t="s">
         <v>21</v>
       </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2" s="2">
-        <v>300000000</v>
-      </c>
-      <c r="M2" s="2">
-        <v>0</v>
-      </c>
       <c r="N2" s="2">
-        <v>50000000</v>
+        <v>0</v>
       </c>
       <c r="O2" s="2">
-        <v>0</v>
+        <v>340000000</v>
       </c>
       <c r="P2" s="2">
-        <v>150000000</v>
+        <v>0</v>
       </c>
       <c r="Q2" s="2">
-        <v>0</v>
+        <v>200000000</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -634,30 +613,6 @@
       <c r="E3" t="s">
         <v>21</v>
       </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="L3" s="2">
-        <v>0</v>
-      </c>
-      <c r="M3" s="2">
-        <v>50000000</v>
-      </c>
       <c r="N3" s="2">
         <v>0</v>
       </c>
@@ -668,7 +623,7 @@
         <v>0</v>
       </c>
       <c r="Q3" s="2">
-        <v>50000000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -687,30 +642,6 @@
       <c r="E4" t="s">
         <v>21</v>
       </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4" s="2">
-        <v>0</v>
-      </c>
-      <c r="M4" s="2">
-        <v>200000000</v>
-      </c>
       <c r="N4" s="2">
         <v>200000000</v>
       </c>
@@ -740,41 +671,17 @@
       <c r="E5" t="s">
         <v>21</v>
       </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5" s="2">
-        <v>50000000</v>
-      </c>
-      <c r="M5" s="2">
-        <v>50000000</v>
-      </c>
       <c r="N5" s="2">
-        <v>60000000</v>
+        <v>30000000</v>
       </c>
       <c r="O5" s="2">
-        <v>60000000</v>
+        <v>35000000</v>
       </c>
       <c r="P5" s="2">
-        <v>70000000</v>
+        <v>0</v>
       </c>
       <c r="Q5" s="2">
-        <v>70000000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -793,41 +700,17 @@
       <c r="E6" t="s">
         <v>22</v>
       </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6" s="2">
-        <v>125000000</v>
-      </c>
-      <c r="M6" s="2">
-        <v>70000000</v>
-      </c>
       <c r="N6" s="2">
-        <v>70000000</v>
+        <v>0</v>
       </c>
       <c r="O6" s="2">
-        <v>70000000</v>
+        <v>40000000</v>
       </c>
       <c r="P6" s="2">
-        <v>125000000</v>
+        <v>0</v>
       </c>
       <c r="Q6" s="2">
-        <v>125000000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -840,47 +723,20 @@
       <c r="C7" t="s">
         <v>28</v>
       </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
       <c r="E7" t="s">
         <v>22</v>
       </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-      <c r="L7" s="2">
-        <v>0</v>
-      </c>
-      <c r="M7" s="2">
-        <v>50000000</v>
-      </c>
       <c r="N7" s="2">
         <v>0</v>
       </c>
       <c r="O7" s="2">
-        <v>50000000</v>
+        <v>0</v>
       </c>
       <c r="P7" s="2">
         <v>0</v>
       </c>
       <c r="Q7" s="2">
-        <v>150000000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -893,47 +749,20 @@
       <c r="C8" t="s">
         <v>29</v>
       </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
       <c r="E8" t="s">
         <v>22</v>
       </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="L8" s="2">
-        <v>0</v>
-      </c>
-      <c r="M8" s="2">
-        <v>50000000</v>
-      </c>
       <c r="N8" s="2">
         <v>0</v>
       </c>
       <c r="O8" s="2">
-        <v>50000000</v>
+        <v>0</v>
       </c>
       <c r="P8" s="2">
         <v>0</v>
       </c>
       <c r="Q8" s="2">
-        <v>150000000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
@@ -944,59 +773,46 @@
         <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="E9" t="s">
         <v>23</v>
       </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-      <c r="J9">
-        <v>0</v>
-      </c>
-      <c r="K9">
-        <v>0</v>
-      </c>
-      <c r="L9" s="2">
-        <v>0</v>
-      </c>
-      <c r="M9" s="2">
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" t="s">
+        <v>23</v>
+      </c>
+      <c r="N10" s="2">
         <v>150000000</v>
       </c>
-      <c r="N9" s="2">
+      <c r="O10" s="2">
         <v>150000000</v>
       </c>
-      <c r="O9" s="2">
+      <c r="P10" s="2">
         <v>150000000</v>
       </c>
-      <c r="P9" s="2">
+      <c r="Q10" s="2">
         <v>150000000</v>
       </c>
-      <c r="Q9" s="2">
-        <v>150000000</v>
-      </c>
-    </row>
-    <row r="82" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D82" s="1"/>
-    </row>
-    <row r="83" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D83" s="1"/>
-    </row>
-    <row r="88" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D88" s="1"/>
+    </row>
+    <row r="80" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D80" s="1"/>
+    </row>
+    <row r="81" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D81" s="1"/>
+    </row>
+    <row r="86" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D86" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>